<commit_message>
added the test data and test method for checkoutasGuest
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\99999.Interview\CoreMintVelvet\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F2DC07-6FC5-493E-B910-3CC3C9A98605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE45DF76-6DC1-4500-87C7-44ED6CF206CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="4665" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3630" yWindow="3300" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Jeans</t>
   </si>
@@ -42,7 +42,16 @@
     <t>searchitem</t>
   </si>
   <si>
-    <t>testnumber</t>
+    <t>checkOutAsGuest</t>
+  </si>
+  <si>
+    <t>Black Bootcut Jeans</t>
+  </si>
+  <si>
+    <t>Shoes</t>
+  </si>
+  <si>
+    <t>Dakota Indigo Washed Jeans</t>
   </si>
 </sst>
 </file>
@@ -360,49 +369,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N3:O4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>12</v>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>